<commit_message>
Course started level 1 lesson 2 completed
</commit_message>
<xml_diff>
--- a/UiPath/ExcelAutomation/MailIDs.xlsx
+++ b/UiPath/ExcelAutomation/MailIDs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="5">
   <si>
     <t>Column1</t>
   </si>
@@ -357,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:A120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,6 +663,306 @@
         <v>2</v>
       </c>
     </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -670,7 +970,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A62"/>
+  <dimension ref="A1:A122"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -683,7 +983,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -984,6 +1284,306 @@
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>